<commit_message>
Update Excel template with latest changes
</commit_message>
<xml_diff>
--- a/api/api/template.xlsx
+++ b/api/api/template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>SMAI CO., LTD</t>
   </si>
@@ -529,18 +529,6 @@
     </r>
   </si>
   <si>
-    <t>FOB Ningbo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TOTAL</t>
-    </r>
     <r>
       <rPr>
         <b/>
@@ -548,16 +536,39 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t>SAY US DOLLARS ONE HUNDRED AND TWENTY-SEVEN THOUSAND TWO HUNDRED ONLY</t>
+      <t>支付条款</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> TERMS OF PAYMENT</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运输路线</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman Regular"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> TRANSPORT ROUTE</t>
     </r>
   </si>
   <si>
@@ -568,93 +579,6 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>支付条款</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> TERMS OF PAYMENT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>付全款提车（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t>100% Payment by T/T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>运输路线</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> TRANSPORT ROUTE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>宁波交车</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Ningbo Delivery</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>运输方式</t>
     </r>
     <r>
@@ -665,24 +589,6 @@
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve"> MODE OF SHIPMENT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>海运</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman Regular"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> Sea</t>
     </r>
   </si>
   <si>
@@ -2556,7 +2462,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2670,9 +2576,6 @@
     </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -3020,89 +2923,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>145415</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>1215390</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1723390</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>741045</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="昇脉公章"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6986905" y="28587065"/>
-          <a:ext cx="1577975" cy="1583055"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>989965</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>484505</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>753745</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2" r:link="rId3">
-          <a:lum contrast="66000"/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2343785" y="29337000"/>
-          <a:ext cx="2119630" cy="845820"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3397,7 +3217,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="149" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="A4" sqref="$A4:$XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -3413,606 +3233,596 @@
   </cols>
   <sheetData>
     <row r="1" ht="51.95" customHeight="1" spans="1:7">
-      <c r="A1" s="60"/>
-      <c r="B1" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="A1" s="59"/>
+      <c r="B1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" s="7" customFormat="1" ht="50.1" customHeight="1" spans="1:8">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="113"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="112"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="39.95" customHeight="1" spans="1:7">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="65" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="114"/>
-      <c r="G3" s="115"/>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="40" customHeight="1" spans="1:7">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65" t="s">
+      <c r="F3" s="113"/>
+      <c r="G3" s="114"/>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="66" customHeight="1" spans="1:7">
+      <c r="A4" s="63"/>
+      <c r="B4" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="116" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="114"/>
-      <c r="G4" s="117"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="116"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="20.25" customHeight="1" spans="1:7">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="65" t="s">
+      <c r="D5" s="68"/>
+      <c r="E5" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="114"/>
-      <c r="G5" s="118"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="117"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="24.75" customHeight="1" spans="1:7">
-      <c r="A6" s="64"/>
-      <c r="B6" s="65" t="s">
+      <c r="A6" s="63"/>
+      <c r="B6" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="119" t="s">
+      <c r="D6" s="69"/>
+      <c r="E6" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="120"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="119"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="81" customHeight="1" spans="1:7">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="121" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="62" customHeight="1" spans="1:7">
-      <c r="A8" s="64"/>
-      <c r="B8" s="65" t="s">
+      <c r="A8" s="63"/>
+      <c r="B8" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="121"/>
-      <c r="F8" s="121"/>
-      <c r="G8" s="121"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="34.5" customHeight="1" spans="1:7">
-      <c r="A9" s="73"/>
-      <c r="B9" s="74" t="s">
+      <c r="A9" s="72"/>
+      <c r="B9" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-    </row>
-    <row r="10" s="59" customFormat="1" ht="71.1" customHeight="1" spans="1:9">
-      <c r="A10" s="75">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+    </row>
+    <row r="10" s="58" customFormat="1" ht="71.1" customHeight="1" spans="1:9">
+      <c r="A10" s="74">
         <v>1</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="122" t="s">
+      <c r="G10" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="133"/>
-    </row>
-    <row r="11" s="59" customFormat="1" ht="48.95" customHeight="1" spans="1:9">
-      <c r="A11" s="75"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="133"/>
-    </row>
-    <row r="12" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A12" s="75"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="133"/>
-    </row>
-    <row r="13" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A13" s="75"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="133"/>
-    </row>
-    <row r="14" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A14" s="75"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="123"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="133"/>
-    </row>
-    <row r="15" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A15" s="75"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="123"/>
-      <c r="G15" s="123"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="133"/>
-    </row>
-    <row r="16" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A16" s="75"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="123"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="133"/>
-    </row>
-    <row r="17" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A17" s="75"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="124"/>
-      <c r="I17" s="133"/>
-    </row>
-    <row r="18" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A18" s="75"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="124"/>
-      <c r="I18" s="133"/>
-    </row>
-    <row r="19" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A19" s="75"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="124"/>
-      <c r="I19" s="133"/>
-    </row>
-    <row r="20" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A20" s="75"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="133"/>
-    </row>
-    <row r="21" s="59" customFormat="1" ht="42" customHeight="1" spans="1:9">
-      <c r="A21" s="75"/>
-      <c r="B21" s="80" t="s">
+      <c r="I10" s="132"/>
+    </row>
+    <row r="11" s="58" customFormat="1" ht="48.95" customHeight="1" spans="1:9">
+      <c r="A11" s="74"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="132"/>
+    </row>
+    <row r="12" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A12" s="74"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="132"/>
+    </row>
+    <row r="13" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A13" s="74"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="132"/>
+    </row>
+    <row r="14" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A14" s="74"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="132"/>
+    </row>
+    <row r="15" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A15" s="74"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="132"/>
+    </row>
+    <row r="16" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A16" s="74"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="122"/>
+      <c r="H16" s="123"/>
+      <c r="I16" s="132"/>
+    </row>
+    <row r="17" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A17" s="74"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="123"/>
+      <c r="I17" s="132"/>
+    </row>
+    <row r="18" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A18" s="74"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
+      <c r="H18" s="123"/>
+      <c r="I18" s="132"/>
+    </row>
+    <row r="19" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A19" s="74"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="122"/>
+      <c r="G19" s="122"/>
+      <c r="H19" s="123"/>
+      <c r="I19" s="132"/>
+    </row>
+    <row r="20" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A20" s="74"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="122"/>
+      <c r="G20" s="122"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="132"/>
+    </row>
+    <row r="21" s="58" customFormat="1" ht="42" customHeight="1" spans="1:9">
+      <c r="A21" s="74"/>
+      <c r="B21" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="125" t="s">
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="123">
+      <c r="G21" s="122">
         <f>SUM(G11:G20)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="124"/>
-      <c r="I21" s="133"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="132"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="40" customHeight="1" spans="1:7">
-      <c r="A22" s="83"/>
-      <c r="B22" s="80" t="s">
+      <c r="A22" s="82"/>
+      <c r="B22" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="126" t="s">
+      <c r="C22" s="80"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="125"/>
+      <c r="G22" s="126">
+        <f>G21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" ht="32.45" customHeight="1" spans="1:7">
+      <c r="A23" s="82"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="128"/>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="33.95" customHeight="1" spans="1:7">
+      <c r="A24" s="82">
+        <v>2</v>
+      </c>
+      <c r="B24" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="127">
-        <f>G21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" s="1" customFormat="1" ht="32.45" customHeight="1" spans="1:7">
-      <c r="A23" s="83"/>
-      <c r="B23" s="84" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+    </row>
+    <row r="25" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A25" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="129"/>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="33.95" customHeight="1" spans="1:7">
-      <c r="A24" s="83">
-        <v>2</v>
-      </c>
-      <c r="B24" s="86" t="s">
+      <c r="B25" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="88" t="s">
+      <c r="C25" s="90"/>
+      <c r="D25" s="91"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+    </row>
+    <row r="26" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
+      <c r="A26" s="74">
+        <v>3.2</v>
+      </c>
+      <c r="B26" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
-      <c r="G24" s="130"/>
-    </row>
-    <row r="25" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A25" s="89" t="s">
+      <c r="C26" s="90"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="130"/>
+      <c r="G26" s="130"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="56" customHeight="1" spans="1:7">
+      <c r="A27" s="94">
+        <v>3.3</v>
+      </c>
+      <c r="B27" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="90" t="s">
+      <c r="C27" s="96"/>
+      <c r="D27" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92" t="s">
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+    </row>
+    <row r="28" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
+      <c r="A28" s="94">
+        <v>3.4</v>
+      </c>
+      <c r="B28" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="131"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="131"/>
-    </row>
-    <row r="26" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
-      <c r="A26" s="75">
-        <v>3.2</v>
-      </c>
-      <c r="B26" s="93" t="s">
+      <c r="C28" s="90"/>
+      <c r="D28" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="94" t="s">
+      <c r="E28" s="130"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+    </row>
+    <row r="29" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
+      <c r="A29" s="94">
+        <v>3.5</v>
+      </c>
+      <c r="B29" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="131"/>
-      <c r="F26" s="131"/>
-      <c r="G26" s="131"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="56" customHeight="1" spans="1:7">
-      <c r="A27" s="95">
-        <v>3.3</v>
-      </c>
-      <c r="B27" s="96" t="s">
+      <c r="C29" s="90"/>
+      <c r="D29" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+    </row>
+    <row r="30" s="1" customFormat="1" ht="20" customHeight="1" spans="1:7">
+      <c r="A30" s="97">
+        <v>4</v>
+      </c>
+      <c r="B30" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="97"/>
-      <c r="D27" s="72" t="s">
+      <c r="C30" s="99"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="100"/>
+      <c r="F30" s="100"/>
+      <c r="G30" s="100"/>
+    </row>
+    <row r="31" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A31" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-    </row>
-    <row r="28" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
-      <c r="A28" s="95">
-        <v>3.4</v>
-      </c>
-      <c r="B28" s="93" t="s">
+      <c r="B31" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92" t="s">
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="90"/>
+    </row>
+    <row r="32" s="1" customFormat="1" ht="41" customHeight="1" spans="1:7">
+      <c r="A32" s="97"/>
+      <c r="B32" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="131"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="131"/>
-    </row>
-    <row r="29" s="1" customFormat="1" ht="23.1" customHeight="1" spans="1:7">
-      <c r="A29" s="95">
-        <v>3.5</v>
-      </c>
-      <c r="B29" s="93" t="s">
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+    </row>
+    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A33" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="91"/>
-      <c r="D29" s="92" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="131"/>
-      <c r="F29" s="131"/>
-      <c r="G29" s="131"/>
-    </row>
-    <row r="30" s="1" customFormat="1" ht="20" customHeight="1" spans="1:7">
-      <c r="A30" s="98">
-        <v>4</v>
-      </c>
-      <c r="B30" s="99" t="s">
+      <c r="B33" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="100"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-    </row>
-    <row r="31" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A31" s="89" t="s">
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="71" customHeight="1" spans="1:7">
+      <c r="A34" s="74"/>
+      <c r="B34" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="102" t="s">
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+    </row>
+    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A35" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-    </row>
-    <row r="32" s="1" customFormat="1" ht="41" customHeight="1" spans="1:7">
-      <c r="A32" s="98"/>
-      <c r="B32" s="103" t="s">
+      <c r="B35" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-    </row>
-    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A33" s="89" t="s">
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+    </row>
+    <row r="36" s="1" customFormat="1" ht="231" customHeight="1" spans="1:7">
+      <c r="A36" s="104"/>
+      <c r="B36" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="102" t="s">
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+    </row>
+    <row r="37" s="1" customFormat="1" ht="153" customHeight="1" spans="1:7">
+      <c r="A37" s="105"/>
+      <c r="B37" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="71" customHeight="1" spans="1:7">
-      <c r="A34" s="75"/>
-      <c r="B34" s="104" t="s">
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+    </row>
+    <row r="38" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A38" s="88" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="100"/>
-      <c r="D34" s="100"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="100"/>
-    </row>
-    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A35" s="89" t="s">
+      <c r="B38" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="90" t="s">
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
+    </row>
+    <row r="39" s="1" customFormat="1" ht="194" customHeight="1" spans="1:7">
+      <c r="A39" s="74"/>
+      <c r="B39" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="91"/>
-    </row>
-    <row r="36" s="1" customFormat="1" ht="231" customHeight="1" spans="1:7">
-      <c r="A36" s="105"/>
-      <c r="B36" s="100" t="s">
+      <c r="C39" s="96"/>
+      <c r="D39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="96"/>
+      <c r="G39" s="96"/>
+    </row>
+    <row r="40" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A40" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="100"/>
-      <c r="D36" s="100"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="100"/>
-    </row>
-    <row r="37" s="1" customFormat="1" ht="153" customHeight="1" spans="1:7">
-      <c r="A37" s="106"/>
-      <c r="B37" s="97" t="s">
+      <c r="B40" s="89" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-    </row>
-    <row r="38" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A38" s="89" t="s">
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="34" customHeight="1" spans="1:7">
+      <c r="A41" s="97"/>
+      <c r="B41" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="90" t="s">
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="96"/>
+      <c r="G41" s="96"/>
+    </row>
+    <row r="42" s="1" customFormat="1" ht="112" customHeight="1" spans="1:7">
+      <c r="A42" s="97"/>
+      <c r="B42" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
-    </row>
-    <row r="39" s="1" customFormat="1" ht="194" customHeight="1" spans="1:7">
-      <c r="A39" s="75"/>
-      <c r="B39" s="74" t="s">
+      <c r="C42" s="96"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="96"/>
+      <c r="G42" s="96"/>
+    </row>
+    <row r="43" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
+      <c r="A43" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="97"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="97"/>
-    </row>
-    <row r="40" s="1" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A40" s="89" t="s">
+      <c r="B43" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="90" t="s">
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+    </row>
+    <row r="44" s="7" customFormat="1" ht="129" customHeight="1" spans="1:7">
+      <c r="A44" s="63"/>
+      <c r="B44" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="34" customHeight="1" spans="1:7">
-      <c r="A41" s="98"/>
-      <c r="B41" s="97" t="s">
+      <c r="C44" s="107"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="107"/>
+      <c r="F44" s="107"/>
+      <c r="G44" s="107"/>
+    </row>
+    <row r="45" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
+      <c r="A45" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="97"/>
-      <c r="D41" s="97"/>
-      <c r="E41" s="97"/>
-      <c r="F41" s="97"/>
-      <c r="G41" s="97"/>
-    </row>
-    <row r="42" s="1" customFormat="1" ht="112" customHeight="1" spans="1:7">
-      <c r="A42" s="98"/>
-      <c r="B42" s="97" t="s">
+      <c r="B45" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="97"/>
-      <c r="D42" s="97"/>
-      <c r="E42" s="97"/>
-      <c r="F42" s="97"/>
-      <c r="G42" s="97"/>
-    </row>
-    <row r="43" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A43" s="89" t="s">
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+    </row>
+    <row r="46" s="7" customFormat="1" ht="18" customHeight="1" spans="1:7">
+      <c r="A46" s="104"/>
+      <c r="B46" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="74" t="s">
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
+    </row>
+    <row r="47" s="7" customFormat="1" ht="64.5" customHeight="1" spans="1:5">
+      <c r="A47" s="109"/>
+      <c r="B47" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-    </row>
-    <row r="44" s="7" customFormat="1" ht="129" customHeight="1" spans="1:7">
-      <c r="A44" s="64"/>
-      <c r="B44" s="107" t="s">
+      <c r="C47" s="111"/>
+      <c r="D47" s="111"/>
+      <c r="E47" s="131" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="108"/>
-      <c r="D44" s="108"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="108"/>
-      <c r="G44" s="108"/>
-    </row>
-    <row r="45" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A45" s="89" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="103" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-    </row>
-    <row r="46" s="7" customFormat="1" ht="18" customHeight="1" spans="1:7">
-      <c r="A46" s="105"/>
-      <c r="B46" s="109" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="109"/>
-      <c r="D46" s="109"/>
-      <c r="E46" s="109"/>
-      <c r="F46" s="109"/>
-      <c r="G46" s="109"/>
-    </row>
-    <row r="47" s="7" customFormat="1" ht="64.5" customHeight="1" spans="1:5">
-      <c r="A47" s="110"/>
-      <c r="B47" s="111" t="s">
-        <v>62</v>
-      </c>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="132" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="48" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A48" s="110"/>
+      <c r="A48" s="109"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -4021,7 +3831,7 @@
       <c r="G48" s="1"/>
     </row>
     <row r="49" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A49" s="110"/>
+      <c r="A49" s="109"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4030,7 +3840,7 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A50" s="110"/>
+      <c r="A50" s="109"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4039,7 +3849,7 @@
       <c r="G50" s="1"/>
     </row>
     <row r="51" s="7" customFormat="1" ht="15" customHeight="1" spans="1:7">
-      <c r="A51" s="110"/>
+      <c r="A51" s="109"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4110,7 +3920,6 @@
     <ignoredError sqref="A25" numberStoredAsText="1"/>
     <ignoredError sqref="G22" unlockedFormula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4121,8 +3930,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
@@ -4141,7 +3950,7 @@
   <sheetData>
     <row r="1" ht="49.5" customHeight="1" spans="1:8">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -4154,7 +3963,7 @@
     <row r="2" s="1" customFormat="1" ht="53.1" customHeight="1" spans="1:8">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="12">
         <f>SC!C3</f>
@@ -4163,7 +3972,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="35"/>
       <c r="F2" s="36" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G2" s="12">
         <f>SC!G3</f>
@@ -4174,7 +3983,7 @@
     <row r="3" s="1" customFormat="1" ht="63" customHeight="1" spans="1:7">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="12">
         <f>SC!C4</f>
@@ -4183,9 +3992,9 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="38">
+        <v>63</v>
+      </c>
+      <c r="G3" s="12">
         <f>SC!G4</f>
         <v>0</v>
       </c>
@@ -4195,11 +4004,11 @@
       <c r="B4" s="11"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="37">
+      <c r="E4" s="38"/>
+      <c r="F4" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="12">
         <f>SC!G5</f>
         <v>0</v>
       </c>
@@ -4208,7 +4017,7 @@
     <row r="5" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C5" s="14" t="str">
         <f>SC!C6</f>
@@ -4216,23 +4025,23 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="42"/>
+      <c r="F5" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="41"/>
       <c r="H5" s="37"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="86.1" customHeight="1" spans="1:8">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C6" s="15">
         <f>SC!C7</f>
         <v>0</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="F6" s="43" t="str">
+      <c r="F6" s="42" t="str">
         <f>SC!E7</f>
         <v>Benificiary Bank
 CHINA CITIC BANK CHONGQING BRANCH
@@ -4241,26 +4050,26 @@
 Benificiary Account: （8111214013100727547）
 Bank Address:  NO. 5, WEST STREET, JIANGBEI CITY, JIANGBEI DISTRICT, CHONGQING</v>
       </c>
-      <c r="G6" s="44"/>
-      <c r="H6" s="45"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="117.95" customHeight="1" spans="1:8">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="44"/>
     </row>
     <row r="8" ht="16.5" customHeight="1" spans="3:8">
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" ht="20.25" customHeight="1" spans="1:8">
       <c r="A9" s="17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -4275,22 +4084,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="49" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" ht="60" customHeight="1" spans="1:7">
@@ -4311,11 +4120,11 @@
         <f>SC!E11</f>
         <v>0</v>
       </c>
-      <c r="F11" s="51">
+      <c r="F11" s="50">
         <f>SC!F11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="50">
         <f>SC!G11</f>
         <v>0</v>
       </c>
@@ -4338,11 +4147,11 @@
         <f>SC!E12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="51">
+      <c r="F12" s="50">
         <f>SC!F12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="50">
         <f>SC!G12</f>
         <v>0</v>
       </c>
@@ -4365,11 +4174,11 @@
         <f>SC!E13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F13" s="50">
         <f>SC!F13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="50">
         <f>SC!G13</f>
         <v>0</v>
       </c>
@@ -4392,11 +4201,11 @@
         <f>SC!E14</f>
         <v>0</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="50">
         <f>SC!F14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="50">
         <f>SC!G14</f>
         <v>0</v>
       </c>
@@ -4419,11 +4228,11 @@
         <f>SC!E15</f>
         <v>0</v>
       </c>
-      <c r="F15" s="51">
+      <c r="F15" s="50">
         <f>SC!F15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G15" s="50">
         <f>SC!G15</f>
         <v>0</v>
       </c>
@@ -4446,11 +4255,11 @@
         <f>SC!E16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="51">
+      <c r="F16" s="50">
         <f>SC!F16</f>
         <v>0</v>
       </c>
-      <c r="G16" s="51">
+      <c r="G16" s="50">
         <f>SC!G16</f>
         <v>0</v>
       </c>
@@ -4473,11 +4282,11 @@
         <f>SC!E16</f>
         <v>0</v>
       </c>
-      <c r="F17" s="51">
+      <c r="F17" s="50">
         <f>SC!F16</f>
         <v>0</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="50">
         <f>SC!G16</f>
         <v>0</v>
       </c>
@@ -4500,11 +4309,11 @@
         <f>SC!E17</f>
         <v>0</v>
       </c>
-      <c r="F18" s="51">
+      <c r="F18" s="50">
         <f>SC!F17</f>
         <v>0</v>
       </c>
-      <c r="G18" s="51">
+      <c r="G18" s="50">
         <f>SC!G17</f>
         <v>0</v>
       </c>
@@ -4527,11 +4336,11 @@
         <f>SC!E18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="51">
+      <c r="F19" s="50">
         <f>SC!F18</f>
         <v>0</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="50">
         <f>SC!G18</f>
         <v>0</v>
       </c>
@@ -4554,11 +4363,11 @@
         <f>SC!E19</f>
         <v>0</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="50">
         <f>SC!F19</f>
         <v>0</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="50">
         <f>SC!G19</f>
         <v>0</v>
       </c>
@@ -4566,31 +4375,31 @@
     <row r="21" s="4" customFormat="1" ht="30" customHeight="1" spans="1:7">
       <c r="A21" s="18"/>
       <c r="B21" s="22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53" t="str">
+      <c r="E21" s="51"/>
+      <c r="F21" s="52">
         <f>SC!F22</f>
-        <v>FOB Ningbo</v>
-      </c>
-      <c r="G21" s="54">
+        <v>0</v>
+      </c>
+      <c r="G21" s="53">
         <f>SC!G22</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" s="4" customFormat="1" ht="30" customHeight="1" spans="1:7">
       <c r="A22" s="18"/>
-      <c r="B22" s="24" t="str">
+      <c r="B22" s="24">
         <f>SC!B23</f>
-        <v>TOTAL：SAY US DOLLARS ONE HUNDRED AND TWENTY-SEVEN THOUSAND TWO HUNDRED ONLY</v>
+        <v>0</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="55"/>
+      <c r="G22" s="54"/>
     </row>
     <row r="23" s="5" customFormat="1" ht="36" customHeight="1" spans="1:7">
       <c r="A23" s="26">
@@ -4601,9 +4410,9 @@
         <v>支付条款 TERMS OF PAYMENT</v>
       </c>
       <c r="C23" s="27"/>
-      <c r="D23" s="27" t="str">
+      <c r="D23" s="27">
         <f>SC!D24</f>
-        <v>付全款提车（100% Payment by T/T）</v>
+        <v>0</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
@@ -4618,14 +4427,14 @@
         <v>运输路线 TRANSPORT ROUTE</v>
       </c>
       <c r="C24" s="29"/>
-      <c r="D24" s="27" t="str">
+      <c r="D24" s="27">
         <f>SC!D25</f>
-        <v>宁波交车 Ningbo Delivery</v>
+        <v>0</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
-      <c r="H24" s="56"/>
+      <c r="H24" s="55"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:8">
       <c r="A25" s="28">
@@ -4636,49 +4445,49 @@
         <v>运输方式 MODE OF SHIPMENT</v>
       </c>
       <c r="C25" s="29"/>
-      <c r="D25" s="27" t="str">
+      <c r="D25" s="27">
         <f>SC!D26</f>
-        <v>海运 Sea</v>
+        <v>0</v>
       </c>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
-      <c r="H25" s="57"/>
+      <c r="H25" s="56"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="38.1" customHeight="1" spans="1:8">
       <c r="A26" s="30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
-      <c r="H26" s="57"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" ht="20.1" customHeight="1" spans="1:8">
       <c r="A27" s="32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
-      <c r="H27" s="58"/>
+      <c r="H27" s="57"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:8">
       <c r="A28" s="32" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -4692,7 +4501,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31"/>

</xml_diff>